<commit_message>
moved dirty files around, added program run column and moved to be first, started making sample ID creator
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E444B7CC-EA87-43E2-AAC6-BA263372B721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A94489-378E-4C05-859C-16B55E200271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
-  <si>
-    <t>Location (lake)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Position in transect</t>
   </si>
@@ -50,12 +47,6 @@
     <t>Waypoint Reference</t>
   </si>
   <si>
-    <t>Surface Type</t>
-  </si>
-  <si>
-    <t>Surface Class</t>
-  </si>
-  <si>
     <t>Sample ID</t>
   </si>
   <si>
@@ -167,32 +158,47 @@
     <t>submerged depth</t>
   </si>
   <si>
-    <t>Start time (hh:mm:ss)</t>
-  </si>
-  <si>
-    <t>Stop Time (hh:mm:ss)</t>
-  </si>
-  <si>
-    <t>Date (yyyy_mm_dd)</t>
-  </si>
-  <si>
-    <t>2020_07_30</t>
-  </si>
-  <si>
     <t>bucket</t>
   </si>
   <si>
-    <t>Program run?</t>
-  </si>
-  <si>
     <t>vault_lake</t>
+  </si>
+  <si>
+    <t>program_run?</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>date_(yyyy-mm-dd)</t>
+  </si>
+  <si>
+    <t>location_(lake)</t>
+  </si>
+  <si>
+    <t>start_time_(hh:mm:ss)</t>
+  </si>
+  <si>
+    <t>stop_time_(hh:mm:ss)</t>
+  </si>
+  <si>
+    <t>surface_type</t>
+  </si>
+  <si>
+    <t>surface_class</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +211,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -251,6 +264,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,200 +582,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
-  <dimension ref="A1:AW2"/>
+  <dimension ref="A1:AW6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="15.5546875" customWidth="1"/>
-    <col min="45" max="45" width="12.88671875" customWidth="1"/>
-    <col min="46" max="46" width="12.6640625" customWidth="1"/>
-    <col min="47" max="47" width="14" customWidth="1"/>
-    <col min="48" max="48" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+    <col min="46" max="46" width="12.88671875" customWidth="1"/>
+    <col min="47" max="47" width="12.6640625" customWidth="1"/>
+    <col min="48" max="48" width="14" customWidth="1"/>
+    <col min="49" max="49" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="3">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44042</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3">
         <v>0.71689814814814812</v>
       </c>
-      <c r="C2" s="3">
+      <c r="E2" s="3">
         <v>0.71909722222222217</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
+        <v>44042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4">
+        <v>44042</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4">
+        <v>44042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>44042</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creates sample ID, start and stop times have to meet hh:mm:ss format, gets ride of trailing time in date column
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A94489-378E-4C05-859C-16B55E200271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FAE3F8-31D2-4152-A0E7-DE7079EAB57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Position in transect</t>
   </si>
@@ -152,18 +152,12 @@
     <t>R_value_used</t>
   </si>
   <si>
-    <t>measurement device</t>
-  </si>
-  <si>
     <t>submerged depth</t>
   </si>
   <si>
     <t>bucket</t>
   </si>
   <si>
-    <t>vault_lake</t>
-  </si>
-  <si>
     <t>program_run?</t>
   </si>
   <si>
@@ -189,6 +183,21 @@
   </si>
   <si>
     <t>surface_class</t>
+  </si>
+  <si>
+    <t>collar</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>measurement_device</t>
+  </si>
+  <si>
+    <t>chamber</t>
+  </si>
+  <si>
+    <t>vault-lake</t>
   </si>
 </sst>
 </file>
@@ -196,7 +205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -264,7 +273,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -582,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
-  <dimension ref="A1:AW6"/>
+  <dimension ref="A1:AX6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,177 +602,180 @@
     <col min="2" max="2" width="13.44140625" style="4" customWidth="1"/>
     <col min="3" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
-    <col min="46" max="46" width="12.88671875" customWidth="1"/>
-    <col min="47" max="47" width="12.6640625" customWidth="1"/>
-    <col min="48" max="48" width="14" customWidth="1"/>
-    <col min="49" max="49" width="12.77734375" customWidth="1"/>
+    <col min="6" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.88671875" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" customWidth="1"/>
+    <col min="47" max="47" width="12.88671875" customWidth="1"/>
+    <col min="48" max="48" width="12.6640625" customWidth="1"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
+    <col min="50" max="50" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4">
         <v>44042</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3">
         <v>0.71689814814814812</v>
@@ -772,36 +784,99 @@
         <v>0.71909722222222217</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>44042</v>
       </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.75856481481481486</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.76076388888888891</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4">
         <v>44042</v>
       </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.80023148148148149</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.80243055555555554</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4">
         <v>44042</v>
       </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.84189814814814812</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.84409722222222217</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>44042</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.88356481481481486</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.88576388888888891</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added submersion depth to master file, made slope analysis separate function
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FAE3F8-31D2-4152-A0E7-DE7079EAB57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65E670-A10E-48AD-8E4E-BBFE698A3F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>Position in transect</t>
   </si>
@@ -152,9 +152,6 @@
     <t>R_value_used</t>
   </si>
   <si>
-    <t>submerged depth</t>
-  </si>
-  <si>
     <t>bucket</t>
   </si>
   <si>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>vault-lake</t>
+  </si>
+  <si>
+    <t>exposed_height</t>
+  </si>
+  <si>
+    <t>submerged_depth</t>
   </si>
 </sst>
 </file>
@@ -591,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
-  <dimension ref="A1:AX6"/>
+  <dimension ref="A1:AY6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,180 +605,183 @@
     <col min="2" max="2" width="13.44140625" style="4" customWidth="1"/>
     <col min="3" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" customWidth="1"/>
-    <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.88671875" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" customWidth="1"/>
-    <col min="47" max="47" width="12.88671875" customWidth="1"/>
-    <col min="48" max="48" width="12.6640625" customWidth="1"/>
-    <col min="49" max="49" width="14" customWidth="1"/>
-    <col min="50" max="50" width="12.77734375" customWidth="1"/>
+    <col min="6" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.44140625" customWidth="1"/>
+    <col min="14" max="14" width="23" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" customWidth="1"/>
+    <col min="48" max="48" width="12.88671875" customWidth="1"/>
+    <col min="49" max="49" width="12.6640625" customWidth="1"/>
+    <col min="50" max="50" width="14" customWidth="1"/>
+    <col min="51" max="51" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>42</v>
       </c>
       <c r="B2" s="4">
         <v>44042</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3">
         <v>0.71689814814814812</v>
@@ -784,21 +790,21 @@
         <v>0.71909722222222217</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>44042</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3">
         <v>0.75856481481481486</v>
@@ -807,21 +813,21 @@
         <v>0.76076388888888891</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
       </c>
       <c r="B4" s="4">
         <v>44042</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3">
         <v>0.80023148148148149</v>
@@ -830,21 +836,21 @@
         <v>0.80243055555555554</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4">
         <v>44042</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3">
         <v>0.84189814814814812</v>
@@ -853,18 +859,18 @@
         <v>0.84409722222222217</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>44042</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3">
         <v>0.88356481481481486</v>
@@ -873,10 +879,10 @@
         <v>0.88576388888888891</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
began to add the pressure data to the file
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65E670-A10E-48AD-8E4E-BBFE698A3F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396D54EB-03CF-4060-8804-B270B645DF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Position in transect</t>
   </si>
@@ -197,10 +197,13 @@
     <t>vault-lake</t>
   </si>
   <si>
-    <t>exposed_height</t>
-  </si>
-  <si>
-    <t>submerged_depth</t>
+    <t>submerged_depth(cm)</t>
+  </si>
+  <si>
+    <t>exposed_height(cm)</t>
+  </si>
+  <si>
+    <t>collar_height(cm)</t>
   </si>
 </sst>
 </file>
@@ -594,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
-  <dimension ref="A1:AY6"/>
+  <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,20 +608,20 @@
     <col min="2" max="2" width="13.44140625" style="4" customWidth="1"/>
     <col min="3" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="25.44140625" customWidth="1"/>
-    <col min="14" max="14" width="23" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" customWidth="1"/>
-    <col min="48" max="48" width="12.88671875" customWidth="1"/>
-    <col min="49" max="49" width="12.6640625" customWidth="1"/>
-    <col min="50" max="50" width="14" customWidth="1"/>
-    <col min="51" max="51" width="12.77734375" customWidth="1"/>
+    <col min="6" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="25.44140625" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="12.88671875" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" customWidth="1"/>
+    <col min="49" max="49" width="12.88671875" customWidth="1"/>
+    <col min="50" max="50" width="12.6640625" customWidth="1"/>
+    <col min="51" max="51" width="14" customWidth="1"/>
+    <col min="52" max="52" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -647,133 +650,136 @@
         <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>54</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -798,8 +804,14 @@
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>34.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>44042</v>
       </c>
@@ -818,8 +830,17 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>34.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -841,8 +862,17 @@
       <c r="I4" t="s">
         <v>50</v>
       </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>34.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -864,8 +894,17 @@
       <c r="I5" t="s">
         <v>50</v>
       </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>34.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>44042</v>
       </c>
@@ -883,6 +922,15 @@
       </c>
       <c r="I6" t="s">
         <v>50</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>34.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes file format to yyyy_mm_dd_hhh_mm M_ssS_location_measurement-device, also changed flux reading in excel table from h^-1 to s^-1
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396D54EB-03CF-4060-8804-B270B645DF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB63B9-1221-44D5-BFDF-70197F7BE1F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Sample ID</t>
   </si>
   <si>
-    <t>mmol CH4 m^-2 hr^-1</t>
-  </si>
-  <si>
     <t>± uncertainty</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>collar_height(cm)</t>
+  </si>
+  <si>
+    <t>mmol CH4 m^-2 s^-1</t>
   </si>
 </sst>
 </file>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
   <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,40 +623,40 @@
   <sheetData>
     <row r="1" spans="1:52" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
@@ -674,120 +674,120 @@
         <v>0</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4">
         <v>44042</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3">
         <v>0.71689814814814812</v>
@@ -796,10 +796,10 @@
         <v>0.71909722222222217</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -816,7 +816,7 @@
         <v>44042</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3">
         <v>0.75856481481481486</v>
@@ -825,10 +825,10 @@
         <v>0.76076388888888891</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -842,13 +842,13 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4">
         <v>44042</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3">
         <v>0.80023148148148149</v>
@@ -857,10 +857,10 @@
         <v>0.80243055555555554</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -874,13 +874,13 @@
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="4">
         <v>44042</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3">
         <v>0.84189814814814812</v>
@@ -889,10 +889,10 @@
         <v>0.84409722222222217</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -909,7 +909,7 @@
         <v>44042</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3">
         <v>0.88356481481481486</v>
@@ -918,10 +918,10 @@
         <v>0.88576388888888891</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6">
         <v>0</v>

</xml_diff>

<commit_message>
changed excel spreadsheet flux error variables, started adding data to master spreadsheet
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB63B9-1221-44D5-BFDF-70197F7BE1F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855005A4-0908-4E63-8D97-97D126FD4A73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Position in transect</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Sample ID</t>
   </si>
   <si>
-    <t>± uncertainty</t>
-  </si>
-  <si>
     <t>R_value</t>
   </si>
   <si>
@@ -203,7 +200,13 @@
     <t>collar_height(cm)</t>
   </si>
   <si>
-    <t>mmol CH4 m^-2 s^-1</t>
+    <t>CH4 flux μmol m^-2 s^-1</t>
+  </si>
+  <si>
+    <t>CH4 flux ± uncertainty</t>
+  </si>
+  <si>
+    <t>CO2 flux ± uncertainty</t>
   </si>
 </sst>
 </file>
@@ -599,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
   <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,40 +626,40 @@
   <sheetData>
     <row r="1" spans="1:52" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
@@ -674,120 +677,120 @@
         <v>0</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4">
         <v>44042</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3">
         <v>0.71689814814814812</v>
@@ -796,10 +799,10 @@
         <v>0.71909722222222217</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -816,7 +819,7 @@
         <v>44042</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3">
         <v>0.75856481481481486</v>
@@ -825,10 +828,10 @@
         <v>0.76076388888888891</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -842,13 +845,13 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4">
         <v>44042</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3">
         <v>0.80023148148148149</v>
@@ -857,10 +860,10 @@
         <v>0.80243055555555554</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -874,13 +877,13 @@
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4">
         <v>44042</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="3">
         <v>0.84189814814814812</v>
@@ -889,10 +892,10 @@
         <v>0.84409722222222217</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -909,7 +912,7 @@
         <v>44042</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="3">
         <v>0.88356481481481486</v>
@@ -918,10 +921,10 @@
         <v>0.88576388888888891</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6">
         <v>0</v>

</xml_diff>

<commit_message>
successfully runs through the times! edits the master data sheet, need to fix so that it doesn't print out the rows to the excel file '
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855005A4-0908-4E63-8D97-97D126FD4A73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4877CB7-9D37-4300-8D3C-7F8CB55A3144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
   <dimension ref="A1:AZ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +784,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4">
         <v>44042</v>

</xml_diff>

<commit_message>
pulls type of gas from excel file
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4877CB7-9D37-4300-8D3C-7F8CB55A3144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A70896-C997-48D4-B0A8-EAFF7263E063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>Position in transect</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>CO2 flux ± uncertainty</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>measurement</t>
   </si>
 </sst>
 </file>
@@ -600,31 +612,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
-  <dimension ref="A1:AZ6"/>
+  <dimension ref="A1:BB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.44140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="25.44140625" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" customWidth="1"/>
-    <col min="49" max="49" width="12.88671875" customWidth="1"/>
-    <col min="50" max="50" width="12.6640625" customWidth="1"/>
-    <col min="51" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="12.77734375" customWidth="1"/>
+    <col min="3" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="7" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="23" max="23" width="15.5546875" customWidth="1"/>
+    <col min="51" max="51" width="12.88671875" customWidth="1"/>
+    <col min="52" max="52" width="12.6640625" customWidth="1"/>
+    <col min="53" max="53" width="14" customWidth="1"/>
+    <col min="54" max="54" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -635,154 +647,160 @@
         <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -792,92 +810,101 @@
       <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="3">
         <v>0.71689814814814812</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>0.71909722222222217</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>39</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>34.5</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
       <c r="B3" s="4">
         <v>44042</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="3">
-        <v>0.75856481481481486</v>
+      <c r="D3" t="s">
+        <v>60</v>
       </c>
       <c r="E3" s="3">
-        <v>0.76076388888888891</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s">
+        <v>0.71689814814814812</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.71909722222222217</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
         <v>39</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>34.5</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>44042</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="3">
-        <v>0.80023148148148149</v>
+      <c r="D4" t="s">
+        <v>59</v>
       </c>
       <c r="E4" s="3">
-        <v>0.80243055555555554</v>
-      </c>
-      <c r="H4" t="s">
+        <v>0.75856481481481486</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.76076388888888891</v>
+      </c>
+      <c r="J4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
+      <c r="K4" t="s">
+        <v>39</v>
       </c>
       <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>34.5</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="4">
         <v>44042</v>
@@ -885,54 +912,95 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="3">
-        <v>0.84189814814814812</v>
+      <c r="D5" t="s">
+        <v>60</v>
       </c>
       <c r="E5" s="3">
-        <v>0.84409722222222217</v>
-      </c>
-      <c r="H5" t="s">
+        <v>0.80023148148148149</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.80243055555555554</v>
+      </c>
+      <c r="J5" t="s">
         <v>50</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>48</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>34.5</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
       <c r="B6" s="4">
         <v>44042</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.84189814814814812</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.84409722222222217</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>44042</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3">
         <v>0.88356481481481486</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F7" s="3">
         <v>0.88576388888888891</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J7" t="s">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K7" t="s">
         <v>48</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <v>34.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bucket_sediment, bucket_chamber are options, trying to get R_sqaured value returned even if the data is rejected
</commit_message>
<xml_diff>
--- a/data/simon_masters.xlsx
+++ b/data/simon_masters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\methane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A70896-C997-48D4-B0A8-EAFF7263E063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A10946-73F3-461A-81B5-20F7B54B7F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F3A828C3-13BB-45BD-8B9E-05D2C1EEBBC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>Position in transect</t>
   </si>
@@ -146,9 +146,6 @@
     <t>R_value_used</t>
   </si>
   <si>
-    <t>bucket</t>
-  </si>
-  <si>
     <t>program_run?</t>
   </si>
   <si>
@@ -219,6 +216,12 @@
   </si>
   <si>
     <t>measurement</t>
+  </si>
+  <si>
+    <t>min sample length</t>
+  </si>
+  <si>
+    <t>bucket_sediment</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87331368-EC89-497D-BBE5-5DF386B0D2B4}">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,182 +639,185 @@
     <col min="54" max="54" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>47</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>48</v>
       </c>
       <c r="B2" s="4">
         <v>44042</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="3">
         <v>0.71689814814814812</v>
@@ -820,10 +826,10 @@
         <v>0.71909722222222217</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -834,19 +840,22 @@
       <c r="N2">
         <v>34.5</v>
       </c>
+      <c r="O2">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4">
         <v>44042</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="3">
         <v>0.71689814814814812</v>
@@ -855,10 +864,10 @@
         <v>0.71909722222222217</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -869,16 +878,19 @@
       <c r="N3">
         <v>34.5</v>
       </c>
+      <c r="O3">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>44042</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3">
         <v>0.75856481481481486</v>
@@ -887,10 +899,10 @@
         <v>0.76076388888888891</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -901,19 +913,22 @@
       <c r="N4">
         <v>34.5</v>
       </c>
+      <c r="O4">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4">
         <v>44042</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3">
         <v>0.80023148148148149</v>
@@ -922,10 +937,10 @@
         <v>0.80243055555555554</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -936,19 +951,22 @@
       <c r="N5">
         <v>34.5</v>
       </c>
+      <c r="O5">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4">
         <v>44042</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3">
         <v>0.84189814814814812</v>
@@ -957,10 +975,10 @@
         <v>0.84409722222222217</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -971,16 +989,19 @@
       <c r="N6">
         <v>34.5</v>
       </c>
+      <c r="O6">
+        <v>45</v>
+      </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>44042</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3">
         <v>0.88356481481481486</v>
@@ -989,10 +1010,10 @@
         <v>0.88576388888888891</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1002,6 +1023,9 @@
       </c>
       <c r="N7">
         <v>34.5</v>
+      </c>
+      <c r="O7">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>